<commit_message>
& - №13862 от 19.10.2024 https://2eurostore.ru/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Lithuania/#EURO#Lithuania#Commemorative#[2015-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Lithuania/#EURO#Lithuania#Commemorative#[2015-present]#UNC%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Lithuania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31774B63-53BD-4F2C-A299-C841B74806A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E895DE3-491F-4D31-A77C-F87079A309E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="1110" windowWidth="28720" windowHeight="19550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="53">
   <si>
     <t>Year</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>The 100th anniversary of the foundation of the independent Baltic states</t>
+  </si>
+  <si>
+    <t>Straw Gardens</t>
   </si>
 </sst>
 </file>
@@ -300,7 +303,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,12 +337,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,7 +434,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
@@ -521,9 +518,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -531,7 +525,7 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -548,6 +542,14 @@
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -919,7 +921,7 @@
       <pane xSplit="9" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1438,29 +1440,25 @@
       <c r="A20" s="22">
         <v>2024</v>
       </c>
-      <c r="B20" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>42</v>
+      <c r="B20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="18">
+        <v>1</v>
       </c>
       <c r="I20" s="7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="I20" si="6">IF(OR(AND(H20&gt;1,H20&lt;&gt;"-")),"Can exchange","")</f>
         <v/>
       </c>
     </row>
@@ -1479,11 +1477,28 @@
     <mergeCell ref="C1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H10">
+    <cfRule type="containsText" dxfId="13" priority="27" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H10">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
     <cfRule type="containsText" dxfId="12" priority="25" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H10">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H11))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1495,12 +1510,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
+  <conditionalFormatting sqref="H12">
     <cfRule type="containsText" dxfId="11" priority="23" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H11))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1512,13 +1527,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12">
-    <cfRule type="containsText" dxfId="10" priority="21" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H12))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12">
-    <cfRule type="colorScale" priority="22">
+  <conditionalFormatting sqref="H13">
+    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -1529,12 +1544,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
+  <conditionalFormatting sqref="H14:H15">
     <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H13))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14:H15">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1546,12 +1561,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14:H15">
+  <conditionalFormatting sqref="H16">
     <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H14))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H14:H15">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1563,13 +1578,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H16))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="H19">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -1580,13 +1595,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H19))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="H17">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H17))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -1597,30 +1612,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
+  <conditionalFormatting sqref="H18">
     <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H17))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
     <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H18))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
-    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -1659,7 +1657,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>